<commit_message>
Dynamic Web Scraper developed. Need to store and analyze the data. And find the metrics.
</commit_message>
<xml_diff>
--- a/hyderabad_restaurants_details.xlsx
+++ b/hyderabad_restaurants_details.xlsx
@@ -73,10 +73,22 @@
     <t>Hyderabad City</t>
   </si>
   <si>
-    <t>Banjara Hills</t>
-  </si>
-  <si>
-    <t>Kothapet</t>
+    <t>Saroor Nagar</t>
+  </si>
+  <si>
+    <t>Nampally</t>
+  </si>
+  <si>
+    <t>RTC X roads</t>
+  </si>
+  <si>
+    <t>Himayath Nagar</t>
+  </si>
+  <si>
+    <t>Lakdikapul</t>
+  </si>
+  <si>
+    <t>Charminar</t>
   </si>
   <si>
     <t>Abids</t>
@@ -85,154 +97,154 @@
     <t>Narayanguda</t>
   </si>
   <si>
-    <t>Charminar</t>
-  </si>
-  <si>
-    <t>Malakpet</t>
-  </si>
-  <si>
-    <t>Somajiguda</t>
-  </si>
-  <si>
-    <t>Nampally</t>
-  </si>
-  <si>
-    <t>Louis Burger</t>
-  </si>
-  <si>
-    <t>Mithaiwala</t>
-  </si>
-  <si>
-    <t>Amay Tiffin Corner</t>
+    <t>Aroma Family Restaurant</t>
+  </si>
+  <si>
+    <t>Nimrah Restaurant</t>
+  </si>
+  <si>
+    <t>Sahara Bakers</t>
+  </si>
+  <si>
+    <t>McDonald's</t>
+  </si>
+  <si>
+    <t>Chicha's</t>
+  </si>
+  <si>
+    <t>Shah Ghouse Hotel &amp; Restaurant</t>
+  </si>
+  <si>
+    <t>Peshawar</t>
+  </si>
+  <si>
+    <t>Krupa Mess &amp; Tiffins</t>
   </si>
   <si>
     <t>Mehfil</t>
   </si>
   <si>
-    <t>Hotel Nayaab</t>
-  </si>
-  <si>
-    <t>The Next Galleria Mall, Malakpet</t>
-  </si>
-  <si>
-    <t>Peshawar</t>
-  </si>
-  <si>
-    <t>Lucky Multicuisine Restaurant</t>
-  </si>
-  <si>
-    <t>Nimrah Restaurant</t>
-  </si>
-  <si>
-    <t>Burger King</t>
-  </si>
-  <si>
-    <t>-</t>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>3.9</t>
+  </si>
+  <si>
+    <t>3.8</t>
+  </si>
+  <si>
+    <t>4.0</t>
   </si>
   <si>
     <t>4.2</t>
   </si>
   <si>
-    <t>3.7</t>
-  </si>
-  <si>
-    <t>4.1</t>
-  </si>
-  <si>
-    <t>4.4</t>
-  </si>
-  <si>
-    <t>3.9</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>510</t>
-  </si>
-  <si>
-    <t>305</t>
-  </si>
-  <si>
-    <t>4,683</t>
-  </si>
-  <si>
-    <t>538</t>
-  </si>
-  <si>
-    <t>253</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>691</t>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>3.4</t>
+  </si>
+  <si>
+    <t>209</t>
   </si>
   <si>
     <t>71</t>
   </si>
   <si>
-    <t>4.0</t>
-  </si>
-  <si>
-    <t>3.8</t>
-  </si>
-  <si>
-    <t>621</t>
-  </si>
-  <si>
-    <t>53</t>
-  </si>
-  <si>
-    <t>23K</t>
-  </si>
-  <si>
-    <t>184.9K</t>
-  </si>
-  <si>
-    <t>4,950</t>
-  </si>
-  <si>
-    <t>12.6K</t>
-  </si>
-  <si>
-    <t>230</t>
-  </si>
-  <si>
-    <t>80.6K</t>
-  </si>
-  <si>
-    <t>402</t>
+    <t>723</t>
+  </si>
+  <si>
+    <t>881</t>
+  </si>
+  <si>
+    <t>1,902</t>
+  </si>
+  <si>
+    <t>3,521</t>
+  </si>
+  <si>
+    <t>807</t>
+  </si>
+  <si>
+    <t>615</t>
+  </si>
+  <si>
+    <t>4,685</t>
+  </si>
+  <si>
+    <t>3.6</t>
+  </si>
+  <si>
+    <t>14.5K</t>
+  </si>
+  <si>
+    <t>461</t>
+  </si>
+  <si>
+    <t>69.1K</t>
+  </si>
+  <si>
+    <t>17.9K</t>
+  </si>
+  <si>
+    <t>306</t>
+  </si>
+  <si>
+    <t>120.4K</t>
+  </si>
+  <si>
+    <t>254</t>
+  </si>
+  <si>
+    <t>40.3K</t>
+  </si>
+  <si>
+    <t>185.3K</t>
+  </si>
+  <si>
+    <t>['Hyderabadi', 'North Indian', 'Chinese', 'Biryani', 'Shawarma']</t>
+  </si>
+  <si>
+    <t>['Bakery', 'Fast Food']</t>
+  </si>
+  <si>
+    <t>['Chinese', 'Bakery', 'Sichuan', 'Pizza', 'Burger', 'Fast Food', 'Desserts']</t>
   </si>
   <si>
     <t>['Burger', 'Fast Food']</t>
   </si>
   <si>
-    <t>['Mithai', 'Bakery', 'Street Food']</t>
-  </si>
-  <si>
-    <t>['South Indian', 'Street Food', 'Juices', 'Beverages']</t>
+    <t>['Kebab', 'Rolls', 'Chinese', 'Biryani', 'Desserts', 'Beverages']</t>
+  </si>
+  <si>
+    <t>['North Indian', 'Mughlai', 'Chinese', 'Mandi', 'Biryani', 'Shawarma', 'Desserts']</t>
+  </si>
+  <si>
+    <t>['North Indian', 'Seafood', 'Kebab', 'Chinese']</t>
+  </si>
+  <si>
+    <t>['South Indian', 'Chinese', 'North Indian', 'Sichuan', 'Pizza']</t>
   </si>
   <si>
     <t>['Kebab', 'Biryani']</t>
   </si>
   <si>
-    <t>['North Indian', 'Mughlai', 'Chinese', 'Beverages']</t>
-  </si>
-  <si>
-    <t>['North Indian', 'Seafood', 'Kebab', 'Chinese']</t>
-  </si>
-  <si>
-    <t>['North Indian', 'Chinese', 'Seafood', 'Mughlai', 'Biryani', 'Shawarma', 'Mandi']</t>
-  </si>
-  <si>
-    <t>['Bakery', 'Fast Food']</t>
-  </si>
-  <si>
-    <t>Banjara Hills, Hyderabad</t>
-  </si>
-  <si>
-    <t>Kothapet, Hyderabad</t>
+    <t>Saroor Nagar, Hyderabad</t>
+  </si>
+  <si>
+    <t>Nampally, Hyderabad</t>
+  </si>
+  <si>
+    <t>RTC X roads, Hyderabad</t>
+  </si>
+  <si>
+    <t>Himayath Nagar, Hyderabad</t>
+  </si>
+  <si>
+    <t>Lakdikapul, Hyderabad</t>
+  </si>
+  <si>
+    <t>Charminar, Hyderabad</t>
   </si>
   <si>
     <t>Abids, Hyderabad</t>
@@ -241,76 +253,64 @@
     <t>Narayanguda, Hyderabad</t>
   </si>
   <si>
-    <t>Charminar, Hyderabad</t>
-  </si>
-  <si>
-    <t>The Next Galleria Mall, Malakpet, Hyderabad</t>
-  </si>
-  <si>
-    <t>Malakpet, Hyderabad</t>
-  </si>
-  <si>
-    <t>Somajiguda, Hyderabad</t>
-  </si>
-  <si>
-    <t>Nampally, Hyderabad</t>
-  </si>
-  <si>
     <t>[]</t>
   </si>
   <si>
+    <t>['Coffee and Doughnuts, Yummy Cake, Choco Chip Cake, Fruit Biscuits, Strawberry Cake, Butterscotch Pastry']</t>
+  </si>
+  <si>
+    <t>['Mc Spicy Chicken, Chocolate Icecreams, Burgers, French Fries']</t>
+  </si>
+  <si>
+    <t>['Lamb Briyani, Keema Masala, Bheja Fry, Red Chicken, Pathar Ka Ghost, Authentic Hyderabadi Food']</t>
+  </si>
+  <si>
+    <t>['Hariyali Chicken, Authentic Hyderabadi Biryani, Mutton Haleem, Plain Rice, Chai, Tandoori Chicken']</t>
+  </si>
+  <si>
     <t>['Jumbo Chicken Biryani, Panneer Butter Masala, Naan, Tea']</t>
   </si>
   <si>
-    <t>['Paya, Khichdi, Keema, Butter Naan, Haleem, Roti']</t>
-  </si>
-  <si>
-    <t>['Cheesecake, Drink, Fries, Chicken Wings']</t>
-  </si>
-  <si>
-    <t>['₹350 for one order (approx.)']</t>
+    <t>['₹700 for two people (approx.)']</t>
+  </si>
+  <si>
+    <t>['₹200 for two people (approx.)']</t>
   </si>
   <si>
     <t>['₹300 for two people (approx.)']</t>
   </si>
   <si>
-    <t>['₹200 for two people (approx.)']</t>
-  </si>
-  <si>
-    <t>['₹700 for two people (approx.)']</t>
-  </si>
-  <si>
-    <t>['₹850 for two people (approx.)']</t>
-  </si>
-  <si>
-    <t>['₹400 for two people (approx.)']</t>
+    <t>['₹500 for two people (approx.)']</t>
+  </si>
+  <si>
+    <t>['₹1,000 for two people (approx.)']</t>
   </si>
   <si>
     <t>['₹1,200 for two people (approx.)']</t>
   </si>
   <si>
-    <t>['₹950 for two people (approx.)']</t>
-  </si>
-  <si>
-    <t>['Delivery Only', 'No Seating Available']</t>
-  </si>
-  <si>
-    <t>['Breakfast', 'Home Delivery', 'Takeaway Available', 'Indoor Seating', 'Desserts and Bakes']</t>
-  </si>
-  <si>
-    <t>['Breakfast', 'Home Delivery', 'Takeaway Available', 'Vegetarian Only', 'Indoor Seating']</t>
+    <t>['Home Delivery', 'Takeaway Available', 'Indoor Seating', 'Family Friendly']</t>
+  </si>
+  <si>
+    <t>['Breakfast', 'Home Delivery', 'Takeaway Available', 'Desserts and Bakes']</t>
+  </si>
+  <si>
+    <t>['Home Delivery', 'Takeaway Available', 'Desserts and Bakes', 'Indoor Seating']</t>
+  </si>
+  <si>
+    <t>['Home Delivery', 'Takeaway Available', 'Indoor Seating']</t>
+  </si>
+  <si>
+    <t>['Home Delivery', 'Takeaway Available', 'Outdoor Seating', 'Family Friendly', 'Indoor Seating', 'Desserts and Bakes']</t>
+  </si>
+  <si>
+    <t>['Home Delivery', 'Takeaway Available', 'Indoor Seating', 'Family Friendly', 'Desserts and Bakes']</t>
+  </si>
+  <si>
+    <t>['Breakfast', 'Home Delivery', 'Takeaway Available', 'Indoor Seating']</t>
   </si>
   <si>
     <t>['Home Delivery', 'Takeaway Available', 'Family Friendly', 'Indoor Seating']</t>
-  </si>
-  <si>
-    <t>['Breakfast', 'Home Delivery', 'Takeaway Available', 'Indoor Seating', 'Family Friendly']</t>
-  </si>
-  <si>
-    <t>['Home Delivery', 'Takeaway Available', 'Mall Parking', 'Indoor Seating']</t>
-  </si>
-  <si>
-    <t>['Breakfast', 'Home Delivery', 'Takeaway Available', 'Desserts and Bakes']</t>
   </si>
 </sst>
 </file>
@@ -744,34 +744,34 @@
         <v>27</v>
       </c>
       <c r="G2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H2" t="s">
         <v>43</v>
       </c>
       <c r="I2" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="J2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L2" t="s">
         <v>71</v>
       </c>
       <c r="M2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -794,34 +794,34 @@
         <v>28</v>
       </c>
       <c r="G3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H3" t="s">
         <v>44</v>
       </c>
       <c r="I3" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="J3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L3" t="s">
         <v>72</v>
       </c>
       <c r="M3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="P3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -844,34 +844,34 @@
         <v>29</v>
       </c>
       <c r="G4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H4" t="s">
         <v>45</v>
       </c>
       <c r="I4" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="J4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L4" t="s">
         <v>73</v>
       </c>
       <c r="M4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N4" t="s">
         <v>80</v>
       </c>
       <c r="O4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="P4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -894,34 +894,34 @@
         <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H5" t="s">
         <v>46</v>
       </c>
       <c r="I5" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="J5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L5" t="s">
         <v>74</v>
       </c>
       <c r="M5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N5" t="s">
         <v>81</v>
       </c>
       <c r="O5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="P5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -944,34 +944,34 @@
         <v>31</v>
       </c>
       <c r="G6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H6" t="s">
         <v>47</v>
       </c>
       <c r="I6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="J6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L6" t="s">
         <v>75</v>
       </c>
       <c r="M6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N6" t="s">
         <v>82</v>
       </c>
       <c r="O6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="P6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -991,7 +991,7 @@
         <v>32</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G7" t="s">
         <v>40</v>
@@ -1003,16 +1003,16 @@
         <v>40</v>
       </c>
       <c r="J7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K7" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="L7" t="s">
         <v>76</v>
       </c>
       <c r="M7" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="N7" t="s">
         <v>83</v>
@@ -1021,7 +1021,7 @@
         <v>89</v>
       </c>
       <c r="P7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1035,7 +1035,7 @@
         <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
         <v>33</v>
@@ -1044,34 +1044,34 @@
         <v>33</v>
       </c>
       <c r="G8" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H8" t="s">
         <v>49</v>
       </c>
       <c r="I8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K8" t="s">
         <v>68</v>
       </c>
       <c r="L8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="M8" t="s">
         <v>68</v>
       </c>
       <c r="N8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O8" t="s">
         <v>90</v>
       </c>
       <c r="P8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1094,34 +1094,34 @@
         <v>34</v>
       </c>
       <c r="G9" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H9" t="s">
         <v>50</v>
       </c>
       <c r="I9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K9" t="s">
         <v>69</v>
       </c>
       <c r="L9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M9" t="s">
         <v>69</v>
       </c>
       <c r="N9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O9" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="P9" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1144,31 +1144,31 @@
         <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H10" t="s">
         <v>51</v>
       </c>
       <c r="I10" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="J10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K10" t="s">
         <v>70</v>
       </c>
       <c r="L10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M10" t="s">
         <v>70</v>
       </c>
       <c r="N10" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="O10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P10" t="s">
         <v>98</v>

</xml_diff>